<commit_message>
Mise à jour du portfolio
</commit_message>
<xml_diff>
--- a/Tableau Synthèse.xlsx
+++ b/Tableau Synthèse.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\betan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\betan\OneDrive\Bureau\PHOTO\Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B63E98-F6FE-4A58-8F56-F5CFC823A83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC38806D-7750-4404-BE18-7D47B0166EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -127,6 +127,24 @@
   <si>
     <t xml:space="preserve">
 </t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestion des tickets GLPI </t>
+  </si>
+  <si>
+    <t>Baie de brassage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Migration de poste </t>
+  </si>
+  <si>
+    <t>OVH/phpMyAdmin</t>
+  </si>
+  <si>
+    <t>Procédure explicative pour résoudre un problème</t>
   </si>
 </sst>
 </file>
@@ -136,7 +154,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -198,6 +216,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -207,7 +237,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -589,6 +619,47 @@
         <color theme="2" tint="-0.749992370372631"/>
       </top>
       <bottom style="medium">
+        <color theme="2" tint="-0.749992370372631"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </left>
+      <right style="medium">
+        <color theme="2" tint="-0.749992370372631"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color theme="2" tint="-0.749992370372631"/>
       </bottom>
       <diagonal/>
@@ -598,7 +669,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -663,9 +734,48 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -690,44 +800,50 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1039,8 +1155,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1053,56 +1169,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="22"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:43" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="29" t="s">
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="30"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="43"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="41"/>
       <c r="F4" s="14" t="s">
         <v>8</v>
       </c>
@@ -1114,22 +1230,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="43"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="31" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1152,8 +1268,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
-      <c r="B7" s="40"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1209,16 +1325,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="35"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="27"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1708,16 +1824,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="38"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="30"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1755,13 +1871,21 @@
       <c r="AQ19"/>
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
+      <c r="A20" s="44" t="s">
+        <v>29</v>
+      </c>
       <c r="B20" s="10"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
+      <c r="C20" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="45" t="s">
+        <v>28</v>
+      </c>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
+      <c r="G20" s="45" t="s">
+        <v>28</v>
+      </c>
       <c r="H20" s="18"/>
       <c r="I20"/>
       <c r="J20"/>
@@ -1800,14 +1924,24 @@
       <c r="AQ20"/>
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+      <c r="A21" s="46" t="s">
+        <v>30</v>
+      </c>
       <c r="B21" s="10"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
+      <c r="C21" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="45" t="s">
+        <v>28</v>
+      </c>
       <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="18"/>
+      <c r="F21" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="H21" s="47"/>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
@@ -1845,13 +1979,23 @@
       <c r="AQ21"/>
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="A22" s="44" t="s">
+        <v>31</v>
+      </c>
       <c r="B22" s="10"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
+      <c r="C22" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="45" t="s">
+        <v>28</v>
+      </c>
       <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
+      <c r="F22" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="45" t="s">
+        <v>28</v>
+      </c>
       <c r="H22" s="18"/>
       <c r="I22"/>
       <c r="J22"/>
@@ -1890,13 +2034,21 @@
       <c r="AQ22"/>
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
+      <c r="A23" s="44" t="s">
+        <v>32</v>
+      </c>
       <c r="B23" s="10"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
+      <c r="C23" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="45" t="s">
+        <v>28</v>
+      </c>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
+      <c r="G23" s="45" t="s">
+        <v>28</v>
+      </c>
       <c r="H23" s="18"/>
       <c r="I23"/>
       <c r="J23"/>
@@ -1935,14 +2087,22 @@
       <c r="AQ23"/>
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="18"/>
+      <c r="A24" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="48"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" s="51"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -1980,14 +2140,20 @@
       <c r="AQ24"/>
     </row>
     <row r="25" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="18"/>
+      <c r="A25" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="55"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="57" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="58" t="s">
+        <v>28</v>
+      </c>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -2026,13 +2192,13 @@
     </row>
     <row r="26" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="18"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="54"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2070,16 +2236,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="38"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="30"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2524,6 +2690,11 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2531,11 +2702,6 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>